<commit_message>
March 2025 Changes & ITNOW
</commit_message>
<xml_diff>
--- a/static/ITNOW/ITNOW_History.xlsx
+++ b/static/ITNOW/ITNOW_History.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaviselli/Documents/MATLAB/IT-NOWCAST/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CC49BB8-2518-E941-A406-AA128424D574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D43B46E-588E-BE4D-A50F-7A1EF72AF17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16960" xr2:uid="{6515F016-35AB-974D-935F-759783D4EEB3}"/>
+    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16960" activeTab="1" xr2:uid="{6515F016-35AB-974D-935F-759783D4EEB3}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Nowcast</t>
   </si>
@@ -113,13 +113,16 @@
       <t xml:space="preserve"> (see the 'Nowcast' sheet)</t>
     </r>
   </si>
+  <si>
+    <t>Preliminary</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -302,20 +305,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -337,12 +338,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -357,6 +352,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -694,80 +698,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90D93CB-F2CC-4846-9043-D3CBF77BCCEB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="11" customWidth="1"/>
-    <col min="2" max="2" width="53" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="11"/>
+    <col min="1" max="1" width="12.83203125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="53" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="11">
         <v>45717</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15"/>
-    </row>
-    <row r="4" spans="1:2" s="18" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="13"/>
+    </row>
+    <row r="4" spans="1:2" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="17"/>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
     </row>
@@ -781,110 +785,133 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB345B88-5858-7445-BD80-F1D8778C0EB0}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="3" customWidth="1"/>
-    <col min="2" max="6" width="12.83203125" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="12.83203125" style="22" customWidth="1"/>
+    <col min="2" max="7" width="12.83203125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45623</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>2.0774979510870002E-3</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>2.18859437226E-3</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="3">
         <v>-7.5776100149673397E-4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>6.3731985397719997E-3</v>
       </c>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45648</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="3">
         <v>1.58897260909078E-4</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>3.2616874401746E-4</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>-2.5979068330139999E-3</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>4.537530056263E-3</v>
       </c>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45674</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>7.1822143680192005E-4</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1.33138092781256E-4</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>-2.7998081995269999E-3</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>4.3451720593169997E-3</v>
       </c>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45688</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>9.7115040231823498E-4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>2.5371042867359899E-4</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>-2.5966240483699999E-3</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>3.679988888085E-3</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="4">
+        <v>-1.5100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="22">
+        <v>45717</v>
+      </c>
+      <c r="B6" s="4">
+        <v>-7.7999999999999996E-3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>-1.3498623600948599E-2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>-1.67080259537454E-2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-9.3160171174270206E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated ITNOW March 2025
</commit_message>
<xml_diff>
--- a/static/ITNOW/ITNOW_History.xlsx
+++ b/static/ITNOW/ITNOW_History.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaviselli/Documents/MATLAB/IT-NOWCAST/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C13746-8C47-2443-94E2-137B94B2F872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70850230-1BAA-FD44-85C1-76C804096A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16960" activeTab="1" xr2:uid="{6515F016-35AB-974D-935F-759783D4EEB3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="10100" xr2:uid="{6515F016-35AB-974D-935F-759783D4EEB3}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Nowcast</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>Realization of GDP growth, quarterly</t>
-  </si>
-  <si>
-    <t>Value of the real-time prediction, monthly</t>
   </si>
   <si>
     <t>5% (lower bound) of the empirical prediction interval, monthly</t>
@@ -115,6 +112,27 @@
   </si>
   <si>
     <t>Preliminary</t>
+  </si>
+  <si>
+    <t>Preliminary Realization of GDP growth, quarterly</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Q4-2024</t>
+  </si>
+  <si>
+    <t>Q1-2025</t>
+  </si>
+  <si>
+    <t>Real-time prediction for GDP growth, monthly</t>
+  </si>
+  <si>
+    <t>Updated prediction for previous month GDP growth, monthly</t>
+  </si>
+  <si>
+    <t>Reference quarter for the nowcast, if relative to a quarter</t>
   </si>
 </sst>
 </file>
@@ -305,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -360,6 +378,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -696,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90D93CB-F2CC-4846-9043-D3CBF77BCCEB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,7 +738,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -731,7 +755,7 @@
     </row>
     <row r="4" spans="1:2" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="22"/>
     </row>
@@ -744,34 +768,58 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
-        <v>0</v>
+      <c r="A6" s="15" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
-        <v>2</v>
+      <c r="A7" s="15" t="s">
+        <v>11</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="B10" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B12" s="19" t="s">
         <v>8</v>
       </c>
     </row>
@@ -785,152 +833,147 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB345B88-5858-7445-BD80-F1D8778C0EB0}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView zoomScale="103" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" style="20" customWidth="1"/>
-    <col min="2" max="7" width="12.83203125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="14.1640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>15</v>
-      </c>
       <c r="G1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45623</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="23"/>
+      <c r="C2" s="3">
         <v>2.0774979510870002E-3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="D2" s="3">
         <v>2.18859437226E-3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>-7.5776100149673397E-4</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>6.3731985397719997E-3</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45648</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="23"/>
+      <c r="C3" s="3">
         <v>1.58897260909078E-4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="3">
         <v>3.2616874401746E-4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>-2.5979068330139999E-3</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>4.537530056263E-3</v>
       </c>
-      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45674</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="4">
         <v>7.1822143680192005E-4</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <v>1.33138092781256E-4</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="4">
         <v>-2.7998081995269999E-3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="4">
         <v>4.3451720593169997E-3</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>45688</v>
-      </c>
-      <c r="B5" s="4">
-        <v>9.7115040231823498E-4</v>
+      <c r="G4" s="4">
+        <v>-1.5100000000000001E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.33E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="20">
+        <v>45717</v>
       </c>
       <c r="C5" s="4">
-        <v>2.5371042867359899E-4</v>
+        <v>-7.7999999999999996E-3</v>
       </c>
       <c r="D5" s="4">
-        <v>-2.5966240483699999E-3</v>
+        <v>-1.3498623600948599E-2</v>
       </c>
       <c r="E5" s="4">
-        <v>3.679988888085E-3</v>
+        <v>-1.67080259537454E-2</v>
       </c>
       <c r="F5" s="4">
-        <v>-1.5100000000000001E-2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1.33E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>-9.3160171174270206E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
-        <v>45717</v>
-      </c>
-      <c r="B6" s="4">
-        <v>-7.7999999999999996E-3</v>
+        <v>45760</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>18</v>
       </c>
       <c r="C6" s="4">
-        <v>-1.3498623600948599E-2</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="D6" s="4">
-        <v>-1.67080259537454E-2</v>
+        <v>5.9999999999999995E-4</v>
       </c>
       <c r="E6" s="4">
-        <v>-9.3160171174270206E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
-        <v>45760</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-2.0999999999999999E-3</v>
-      </c>
-      <c r="E7" s="4">
-        <v>4.5999999999999999E-3</v>
+        <v>-2.5999999999999999E-3</v>
+      </c>
+      <c r="F6" s="4">
+        <v>4.7999999999999996E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ITNOW May 2025 Update
</commit_message>
<xml_diff>
--- a/static/ITNOW/ITNOW_History.xlsx
+++ b/static/ITNOW/ITNOW_History.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreaviselli/Documents/MATLAB/IT-NOWCAST/DATA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70850230-1BAA-FD44-85C1-76C804096A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBE03D9-C988-C644-B04D-478D6D79FA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="10100" xr2:uid="{6515F016-35AB-974D-935F-759783D4EEB3}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="10100" activeTab="1" xr2:uid="{6515F016-35AB-974D-935F-759783D4EEB3}"/>
   </bookViews>
   <sheets>
     <sheet name="INFO" sheetId="2" r:id="rId1"/>
@@ -139,9 +139,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000%"/>
-  </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -329,12 +326,6 @@
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -373,16 +364,22 @@
     <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="5" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="6" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -722,104 +719,104 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D90D93CB-F2CC-4846-9043-D3CBF77BCCEB}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="53" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="1" width="12.83203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="53" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>45717</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="13"/>
-    </row>
-    <row r="4" spans="1:2" s="14" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:2" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="22"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -833,43 +830,43 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB345B88-5858-7445-BD80-F1D8778C0EB0}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="24" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -877,103 +874,131 @@
       <c r="A2" s="2">
         <v>45623</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="3">
+      <c r="B2" s="19"/>
+      <c r="C2" s="23">
         <v>2.0774979510870002E-3</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="23">
         <v>2.18859437226E-3</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="23">
         <v>-7.5776100149673397E-4</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="23">
         <v>6.3731985397719997E-3</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45648</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="3">
+      <c r="B3" s="19"/>
+      <c r="C3" s="23">
         <v>1.58897260909078E-4</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="23">
         <v>3.2616874401746E-4</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="23">
         <v>-2.5979068330139999E-3</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="23">
         <v>4.537530056263E-3</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45674</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="24">
         <v>7.1822143680192005E-4</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="24">
         <v>1.33138092781256E-4</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="24">
         <v>-2.7998081995269999E-3</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="24">
         <v>4.3451720593169997E-3</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="24">
         <v>-1.5100000000000001E-2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="24">
         <v>1.33E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="A5" s="18">
         <v>45717</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="24">
         <v>-7.7999999999999996E-3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="24">
         <v>-1.3498623600948599E-2</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="24">
         <v>-1.67080259537454E-2</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="24">
         <v>-9.3160171174270206E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="A6" s="18">
         <v>45760</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="24">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="24">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="24">
         <v>-2.5999999999999999E-3</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="24">
         <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="G6" s="24">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H6" s="24">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
+        <v>45787</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
+        <v>45822</v>
+      </c>
+      <c r="C8" s="24">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="D8" s="24">
+        <v>1.4E-3</v>
+      </c>
+      <c r="E8" s="24">
+        <v>-1.6000000000000001E-3</v>
+      </c>
+      <c r="F8" s="24">
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>